<commit_message>
theta method of update
</commit_message>
<xml_diff>
--- a/conejo/output_test.xlsx
+++ b/conejo/output_test.xlsx
@@ -906,7 +906,7 @@
         <v>100</v>
       </c>
       <c r="C43" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -917,7 +917,7 @@
         <v>100</v>
       </c>
       <c r="C44" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="45">
@@ -1547,7 +1547,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F126"/>
+  <dimension ref="A1:F121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1810,10 +1810,10 @@
         <v>175</v>
       </c>
       <c r="C13" t="n">
-        <v>-60.130019</v>
+        <v>3.6946489</v>
       </c>
       <c r="D13" t="n">
-        <v>3.3907669</v>
+        <v>0.70999227</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -1830,10 +1830,10 @@
         <v>175</v>
       </c>
       <c r="C14" t="n">
-        <v>-27.313038</v>
+        <v>-60.130019</v>
       </c>
       <c r="D14" t="n">
-        <v>-4.1183988</v>
+        <v>3.3907669</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -1847,13 +1847,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>400</v>
+        <v>175</v>
       </c>
       <c r="C15" t="n">
-        <v>-162.98913</v>
+        <v>-27.313038</v>
       </c>
       <c r="D15" t="n">
-        <v>-3.1245487</v>
+        <v>-4.1183988</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
@@ -1870,10 +1870,10 @@
         <v>400</v>
       </c>
       <c r="C16" t="n">
-        <v>-200.5349</v>
+        <v>-162.98913</v>
       </c>
       <c r="D16" t="n">
-        <v>-3.250397</v>
+        <v>-3.1245487</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
@@ -1890,10 +1890,10 @@
         <v>400</v>
       </c>
       <c r="C17" t="n">
-        <v>-227.45106</v>
+        <v>-200.5349</v>
       </c>
       <c r="D17" t="n">
-        <v>4.384617</v>
+        <v>-3.250397</v>
       </c>
       <c r="E17" t="n">
         <v>0</v>
@@ -1910,10 +1910,10 @@
         <v>400</v>
       </c>
       <c r="C18" t="n">
-        <v>-264.99683</v>
+        <v>-227.45106</v>
       </c>
       <c r="D18" t="n">
-        <v>4.2587687</v>
+        <v>4.384617</v>
       </c>
       <c r="E18" t="n">
         <v>0</v>
@@ -1927,13 +1927,13 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="C19" t="n">
-        <v>-291.80213</v>
+        <v>-264.99683</v>
       </c>
       <c r="D19" t="n">
-        <v>0.12494801</v>
+        <v>4.2587687</v>
       </c>
       <c r="E19" t="n">
         <v>0</v>
@@ -1950,10 +1950,10 @@
         <v>500</v>
       </c>
       <c r="C20" t="n">
-        <v>-98.63806599999999</v>
+        <v>-291.80213</v>
       </c>
       <c r="D20" t="n">
-        <v>0.52070462</v>
+        <v>0.12494801</v>
       </c>
       <c r="E20" t="n">
         <v>0</v>
@@ -1970,10 +1970,10 @@
         <v>500</v>
       </c>
       <c r="C21" t="n">
-        <v>-226.09704</v>
+        <v>-98.63806599999999</v>
       </c>
       <c r="D21" t="n">
-        <v>0.25079626</v>
+        <v>0.52070462</v>
       </c>
       <c r="E21" t="n">
         <v>0</v>
@@ -1990,10 +1990,10 @@
         <v>500</v>
       </c>
       <c r="C22" t="n">
-        <v>-239.43469</v>
+        <v>-226.09704</v>
       </c>
       <c r="D22" t="n">
-        <v>0.6576118399999999</v>
+        <v>0.25079626</v>
       </c>
       <c r="E22" t="n">
         <v>0</v>
@@ -2010,10 +2010,10 @@
         <v>500</v>
       </c>
       <c r="C23" t="n">
-        <v>-142.21273</v>
+        <v>-239.43469</v>
       </c>
       <c r="D23" t="n">
-        <v>0.40681558</v>
+        <v>0.6576118399999999</v>
       </c>
       <c r="E23" t="n">
         <v>0</v>
@@ -2030,10 +2030,10 @@
         <v>500</v>
       </c>
       <c r="C24" t="n">
-        <v>-292.63807</v>
+        <v>-142.21273</v>
       </c>
       <c r="D24" t="n">
-        <v>0.7314660200000001</v>
+        <v>0.40681558</v>
       </c>
       <c r="E24" t="n">
         <v>0</v>
@@ -2050,10 +2050,10 @@
         <v>500</v>
       </c>
       <c r="C25" t="n">
-        <v>-3.2125197</v>
+        <v>-49.686438</v>
       </c>
       <c r="D25" t="n">
-        <v>-0.38170698</v>
+        <v>0.23639732</v>
       </c>
       <c r="E25" t="n">
         <v>0</v>
@@ -2070,10 +2070,10 @@
         <v>500</v>
       </c>
       <c r="C26" t="n">
-        <v>-210.33898</v>
+        <v>-292.63807</v>
       </c>
       <c r="D26" t="n">
-        <v>-0.21956352</v>
+        <v>0.7314660200000001</v>
       </c>
       <c r="E26" t="n">
         <v>0</v>
@@ -2090,10 +2090,10 @@
         <v>500</v>
       </c>
       <c r="C27" t="n">
-        <v>-210.33898</v>
+        <v>-3.2125197</v>
       </c>
       <c r="D27" t="n">
-        <v>-0.21956352</v>
+        <v>-0.38170698</v>
       </c>
       <c r="E27" t="n">
         <v>0</v>
@@ -2110,10 +2110,10 @@
         <v>500</v>
       </c>
       <c r="C28" t="n">
-        <v>261.89049</v>
+        <v>-210.33898</v>
       </c>
       <c r="D28" t="n">
-        <v>1.6335867</v>
+        <v>-0.21956352</v>
       </c>
       <c r="E28" t="n">
         <v>0</v>
@@ -2130,10 +2130,10 @@
         <v>500</v>
       </c>
       <c r="C29" t="n">
-        <v>-278.78457</v>
+        <v>-210.33898</v>
       </c>
       <c r="D29" t="n">
-        <v>0.08541646899999999</v>
+        <v>-0.21956352</v>
       </c>
       <c r="E29" t="n">
         <v>0</v>
@@ -2150,10 +2150,10 @@
         <v>500</v>
       </c>
       <c r="C30" t="n">
-        <v>37.933983</v>
+        <v>261.89049</v>
       </c>
       <c r="D30" t="n">
-        <v>-0.30684004</v>
+        <v>1.6335867</v>
       </c>
       <c r="E30" t="n">
         <v>0</v>
@@ -2170,10 +2170,10 @@
         <v>500</v>
       </c>
       <c r="C31" t="n">
-        <v>-143.50365</v>
+        <v>-278.78457</v>
       </c>
       <c r="D31" t="n">
-        <v>0.039784363</v>
+        <v>0.08541646899999999</v>
       </c>
       <c r="E31" t="n">
         <v>0</v>
@@ -2190,10 +2190,10 @@
         <v>500</v>
       </c>
       <c r="C32" t="n">
-        <v>-135.28092</v>
+        <v>37.933983</v>
       </c>
       <c r="D32" t="n">
-        <v>0.046568402</v>
+        <v>-0.30684004</v>
       </c>
       <c r="E32" t="n">
         <v>0</v>
@@ -2210,10 +2210,10 @@
         <v>500</v>
       </c>
       <c r="C33" t="n">
-        <v>-38.251826</v>
+        <v>-143.50365</v>
       </c>
       <c r="D33" t="n">
-        <v>0.036942623</v>
+        <v>0.039784363</v>
       </c>
       <c r="E33" t="n">
         <v>0</v>
@@ -2230,10 +2230,10 @@
         <v>500</v>
       </c>
       <c r="C34" t="n">
-        <v>-38.251826</v>
+        <v>-135.28092</v>
       </c>
       <c r="D34" t="n">
-        <v>0.036942623</v>
+        <v>0.046568402</v>
       </c>
       <c r="E34" t="n">
         <v>0</v>
@@ -2250,10 +2250,10 @@
         <v>500</v>
       </c>
       <c r="C35" t="n">
-        <v>-71.533008</v>
+        <v>-38.251826</v>
       </c>
       <c r="D35" t="n">
-        <v>-0.26681743</v>
+        <v>0.036942623</v>
       </c>
       <c r="E35" t="n">
         <v>0</v>
@@ -2270,10 +2270,10 @@
         <v>500</v>
       </c>
       <c r="C36" t="n">
-        <v>-71.533008</v>
+        <v>-38.251826</v>
       </c>
       <c r="D36" t="n">
-        <v>-0.26681743</v>
+        <v>0.036942623</v>
       </c>
       <c r="E36" t="n">
         <v>0</v>
@@ -2290,10 +2290,10 @@
         <v>500</v>
       </c>
       <c r="C37" t="n">
-        <v>-135.53301</v>
+        <v>-71.533008</v>
       </c>
       <c r="D37" t="n">
-        <v>-0.14674958</v>
+        <v>-0.26681743</v>
       </c>
       <c r="E37" t="n">
         <v>0</v>
@@ -2310,10 +2310,10 @@
         <v>500</v>
       </c>
       <c r="C38" t="n">
-        <v>-135.53301</v>
+        <v>-71.533008</v>
       </c>
       <c r="D38" t="n">
-        <v>-0.14674958</v>
+        <v>-0.26681743</v>
       </c>
       <c r="E38" t="n">
         <v>0</v>
@@ -2330,10 +2330,10 @@
         <v>500</v>
       </c>
       <c r="C39" t="n">
-        <v>-164.71908</v>
+        <v>-135.53301</v>
       </c>
       <c r="D39" t="n">
-        <v>-0.030158584</v>
+        <v>-0.14674958</v>
       </c>
       <c r="E39" t="n">
         <v>0</v>
@@ -2347,13 +2347,13 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>175</v>
+        <v>500</v>
       </c>
       <c r="C40" t="n">
-        <v>24.990052</v>
+        <v>-135.53301</v>
       </c>
       <c r="D40" t="n">
-        <v>0.36713513</v>
+        <v>-0.14674958</v>
       </c>
       <c r="E40" t="n">
         <v>0</v>
@@ -2367,13 +2367,13 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>175</v>
+        <v>500</v>
       </c>
       <c r="C41" t="n">
-        <v>-91.732021</v>
+        <v>-164.71908</v>
       </c>
       <c r="D41" t="n">
-        <v>-1.8189607</v>
+        <v>-0.030158584</v>
       </c>
       <c r="E41" t="n">
         <v>0</v>
@@ -2387,13 +2387,13 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>175</v>
+        <v>500</v>
       </c>
       <c r="C42" t="n">
-        <v>-41.25803</v>
+        <v>7.2865617</v>
       </c>
       <c r="D42" t="n">
-        <v>-1.496278</v>
+        <v>-0.13951417</v>
       </c>
       <c r="E42" t="n">
         <v>0</v>
@@ -2410,10 +2410,10 @@
         <v>175</v>
       </c>
       <c r="C43" t="n">
-        <v>-50.509948</v>
+        <v>24.990052</v>
       </c>
       <c r="D43" t="n">
-        <v>-1.3083064</v>
+        <v>0.36713513</v>
       </c>
       <c r="E43" t="n">
         <v>0</v>
@@ -2430,10 +2430,10 @@
         <v>175</v>
       </c>
       <c r="C44" t="n">
-        <v>-21.5</v>
+        <v>-91.732021</v>
       </c>
       <c r="D44" t="n">
-        <v>7.012908</v>
+        <v>-1.8189607</v>
       </c>
       <c r="E44" t="n">
         <v>0</v>
@@ -2450,10 +2450,10 @@
         <v>175</v>
       </c>
       <c r="C45" t="n">
-        <v>2.8699097</v>
+        <v>-41.25803</v>
       </c>
       <c r="D45" t="n">
-        <v>-0.19357947</v>
+        <v>-1.496278</v>
       </c>
       <c r="E45" t="n">
         <v>0</v>
@@ -2467,13 +2467,13 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>400</v>
+        <v>175</v>
       </c>
       <c r="C46" t="n">
-        <v>-270.90728</v>
+        <v>-50.509948</v>
       </c>
       <c r="D46" t="n">
-        <v>-0.21706095</v>
+        <v>-1.3083064</v>
       </c>
       <c r="E46" t="n">
         <v>0</v>
@@ -2490,10 +2490,10 @@
         <v>175</v>
       </c>
       <c r="C47" t="n">
-        <v>-124.50995</v>
+        <v>-21.5</v>
       </c>
       <c r="D47" t="n">
-        <v>-1.071369</v>
+        <v>7.012908</v>
       </c>
       <c r="E47" t="n">
         <v>0</v>
@@ -2510,10 +2510,10 @@
         <v>175</v>
       </c>
       <c r="C48" t="n">
-        <v>-112.25803</v>
+        <v>2.8699097</v>
       </c>
       <c r="D48" t="n">
-        <v>-1.5490878</v>
+        <v>-0.19357947</v>
       </c>
       <c r="E48" t="n">
         <v>0</v>
@@ -2527,16 +2527,16 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>175</v>
+        <v>400</v>
       </c>
       <c r="C49" t="n">
-        <v>-157.5</v>
+        <v>-270.90728</v>
       </c>
       <c r="D49" t="n">
-        <v>2.2280593</v>
+        <v>-0.21706095</v>
       </c>
       <c r="E49" t="n">
-        <v>12.653468</v>
+        <v>0</v>
       </c>
       <c r="F49" t="n">
         <v>0</v>
@@ -2550,10 +2550,10 @@
         <v>175</v>
       </c>
       <c r="C50" t="n">
-        <v>54.928628</v>
+        <v>-124.50995</v>
       </c>
       <c r="D50" t="n">
-        <v>0</v>
+        <v>-1.071369</v>
       </c>
       <c r="E50" t="n">
         <v>0</v>
@@ -2570,10 +2570,10 @@
         <v>175</v>
       </c>
       <c r="C51" t="n">
-        <v>-75.09113499999999</v>
+        <v>-112.25803</v>
       </c>
       <c r="D51" t="n">
-        <v>0.5164128</v>
+        <v>-1.5490878</v>
       </c>
       <c r="E51" t="n">
         <v>0</v>
@@ -2590,13 +2590,13 @@
         <v>175</v>
       </c>
       <c r="C52" t="n">
-        <v>-40.980238</v>
+        <v>-157.5</v>
       </c>
       <c r="D52" t="n">
-        <v>-0.5164128</v>
+        <v>2.2280593</v>
       </c>
       <c r="E52" t="n">
-        <v>0</v>
+        <v>12.653468</v>
       </c>
       <c r="F52" t="n">
         <v>0</v>
@@ -2607,13 +2607,13 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>400</v>
+        <v>175</v>
       </c>
       <c r="C53" t="n">
-        <v>-166.80027</v>
+        <v>54.928628</v>
       </c>
       <c r="D53" t="n">
-        <v>-0.37446351</v>
+        <v>0</v>
       </c>
       <c r="E53" t="n">
         <v>0</v>
@@ -2627,13 +2627,13 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>400</v>
+        <v>175</v>
       </c>
       <c r="C54" t="n">
-        <v>-204.9309</v>
+        <v>-75.09113499999999</v>
       </c>
       <c r="D54" t="n">
-        <v>-0.36461625</v>
+        <v>0.5164128</v>
       </c>
       <c r="E54" t="n">
         <v>0</v>
@@ -2647,13 +2647,13 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>400</v>
+        <v>175</v>
       </c>
       <c r="C55" t="n">
-        <v>-233.80382</v>
+        <v>-40.980238</v>
       </c>
       <c r="D55" t="n">
-        <v>0.6583621</v>
+        <v>-0.5164128</v>
       </c>
       <c r="E55" t="n">
         <v>0</v>
@@ -2670,10 +2670,10 @@
         <v>400</v>
       </c>
       <c r="C56" t="n">
-        <v>-271.93445</v>
+        <v>-166.80027</v>
       </c>
       <c r="D56" t="n">
-        <v>0.66820936</v>
+        <v>-0.37446351</v>
       </c>
       <c r="E56" t="n">
         <v>0</v>
@@ -2687,13 +2687,13 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="C57" t="n">
-        <v>-282.44193</v>
+        <v>-204.9309</v>
       </c>
       <c r="D57" t="n">
-        <v>0.059913155</v>
+        <v>-0.36461625</v>
       </c>
       <c r="E57" t="n">
         <v>0</v>
@@ -2707,13 +2707,13 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="C58" t="n">
-        <v>-118.16215</v>
+        <v>-233.80382</v>
       </c>
       <c r="D58" t="n">
-        <v>0.089525284</v>
+        <v>0.6583621</v>
       </c>
       <c r="E58" t="n">
         <v>0</v>
@@ -2727,13 +2727,13 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="C59" t="n">
-        <v>-215.71332</v>
+        <v>-271.93445</v>
       </c>
       <c r="D59" t="n">
-        <v>0.050065896</v>
+        <v>0.66820936</v>
       </c>
       <c r="E59" t="n">
         <v>0</v>
@@ -2750,10 +2750,10 @@
         <v>500</v>
       </c>
       <c r="C60" t="n">
-        <v>-261.15203</v>
+        <v>-282.44193</v>
       </c>
       <c r="D60" t="n">
-        <v>0.24940293</v>
+        <v>0.059913155</v>
       </c>
       <c r="E60" t="n">
         <v>0</v>
@@ -2770,10 +2770,10 @@
         <v>500</v>
       </c>
       <c r="C61" t="n">
-        <v>-172.15526</v>
+        <v>-118.16215</v>
       </c>
       <c r="D61" t="n">
-        <v>0.19933703</v>
+        <v>0.089525284</v>
       </c>
       <c r="E61" t="n">
         <v>0</v>
@@ -2790,10 +2790,10 @@
         <v>500</v>
       </c>
       <c r="C62" t="n">
-        <v>-312.16215</v>
+        <v>-215.71332</v>
       </c>
       <c r="D62" t="n">
-        <v>0.12576171</v>
+        <v>0.050065896</v>
       </c>
       <c r="E62" t="n">
         <v>0</v>
@@ -2810,10 +2810,10 @@
         <v>500</v>
       </c>
       <c r="C63" t="n">
-        <v>-12.158259</v>
+        <v>-261.15203</v>
       </c>
       <c r="D63" t="n">
-        <v>-0.0013239695</v>
+        <v>0.24940293</v>
       </c>
       <c r="E63" t="n">
         <v>0</v>
@@ -2830,10 +2830,10 @@
         <v>500</v>
       </c>
       <c r="C64" t="n">
-        <v>-235.21773</v>
+        <v>-172.15526</v>
       </c>
       <c r="D64" t="n">
-        <v>0.015821756</v>
+        <v>0.19933703</v>
       </c>
       <c r="E64" t="n">
         <v>0</v>
@@ -2850,10 +2850,10 @@
         <v>500</v>
       </c>
       <c r="C65" t="n">
-        <v>-235.21773</v>
+        <v>-312.16215</v>
       </c>
       <c r="D65" t="n">
-        <v>0.015821756</v>
+        <v>0.12576171</v>
       </c>
       <c r="E65" t="n">
         <v>0</v>
@@ -2870,10 +2870,10 @@
         <v>500</v>
       </c>
       <c r="C66" t="n">
-        <v>270.90728</v>
+        <v>-12.158259</v>
       </c>
       <c r="D66" t="n">
-        <v>0.13437106</v>
+        <v>-0.0013239695</v>
       </c>
       <c r="E66" t="n">
         <v>0</v>
@@ -2890,10 +2890,10 @@
         <v>500</v>
       </c>
       <c r="C67" t="n">
-        <v>-303.8511</v>
+        <v>-235.21773</v>
       </c>
       <c r="D67" t="n">
-        <v>0.032228057</v>
+        <v>0.015821756</v>
       </c>
       <c r="E67" t="n">
         <v>0</v>
@@ -2910,10 +2910,10 @@
         <v>500</v>
       </c>
       <c r="C68" t="n">
-        <v>34.530689</v>
+        <v>-235.21773</v>
       </c>
       <c r="D68" t="n">
-        <v>0.018725063</v>
+        <v>0.015821756</v>
       </c>
       <c r="E68" t="n">
         <v>0</v>
@@ -2930,10 +2930,10 @@
         <v>500</v>
       </c>
       <c r="C69" t="n">
-        <v>-158.88333</v>
+        <v>270.90728</v>
       </c>
       <c r="D69" t="n">
-        <v>-0.0078204681</v>
+        <v>0.13437106</v>
       </c>
       <c r="E69" t="n">
         <v>0</v>
@@ -2950,10 +2950,10 @@
         <v>500</v>
       </c>
       <c r="C70" t="n">
-        <v>-137.68121</v>
+        <v>-303.8511</v>
       </c>
       <c r="D70" t="n">
-        <v>-0.009154016100000001</v>
+        <v>0.032228057</v>
       </c>
       <c r="E70" t="n">
         <v>0</v>
@@ -2970,10 +2970,10 @@
         <v>500</v>
       </c>
       <c r="C71" t="n">
-        <v>-45.941663</v>
+        <v>34.530689</v>
       </c>
       <c r="D71" t="n">
-        <v>-0.0072618632</v>
+        <v>0.018725063</v>
       </c>
       <c r="E71" t="n">
         <v>0</v>
@@ -2990,10 +2990,10 @@
         <v>500</v>
       </c>
       <c r="C72" t="n">
-        <v>-45.941663</v>
+        <v>-158.88333</v>
       </c>
       <c r="D72" t="n">
-        <v>-0.0072618632</v>
+        <v>-0.0078204681</v>
       </c>
       <c r="E72" t="n">
         <v>0</v>
@@ -3010,10 +3010,10 @@
         <v>500</v>
       </c>
       <c r="C73" t="n">
-        <v>-73.234656</v>
+        <v>-137.68121</v>
       </c>
       <c r="D73" t="n">
-        <v>0.016282663</v>
+        <v>-0.009154016100000001</v>
       </c>
       <c r="E73" t="n">
         <v>0</v>
@@ -3030,10 +3030,10 @@
         <v>500</v>
       </c>
       <c r="C74" t="n">
-        <v>-73.234656</v>
+        <v>-45.941663</v>
       </c>
       <c r="D74" t="n">
-        <v>0.016282663</v>
+        <v>-0.0072618632</v>
       </c>
       <c r="E74" t="n">
         <v>0</v>
@@ -3050,10 +3050,10 @@
         <v>500</v>
       </c>
       <c r="C75" t="n">
-        <v>-137.23466</v>
+        <v>-45.941663</v>
       </c>
       <c r="D75" t="n">
-        <v>0.0089554649</v>
+        <v>-0.0072618632</v>
       </c>
       <c r="E75" t="n">
         <v>0</v>
@@ -3070,10 +3070,10 @@
         <v>500</v>
       </c>
       <c r="C76" t="n">
-        <v>-137.23466</v>
+        <v>-73.234656</v>
       </c>
       <c r="D76" t="n">
-        <v>0.0089554649</v>
+        <v>0.016282663</v>
       </c>
       <c r="E76" t="n">
         <v>0</v>
@@ -3090,10 +3090,10 @@
         <v>500</v>
       </c>
       <c r="C77" t="n">
-        <v>-162.31879</v>
+        <v>-73.234656</v>
       </c>
       <c r="D77" t="n">
-        <v>0.0059283152</v>
+        <v>0.016282663</v>
       </c>
       <c r="E77" t="n">
         <v>0</v>
@@ -3107,13 +3107,13 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>175</v>
+        <v>500</v>
       </c>
       <c r="C78" t="n">
-        <v>24.990052</v>
+        <v>-137.23466</v>
       </c>
       <c r="D78" t="n">
-        <v>1.2938696</v>
+        <v>0.0089554649</v>
       </c>
       <c r="E78" t="n">
         <v>0</v>
@@ -3127,13 +3127,13 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>175</v>
+        <v>500</v>
       </c>
       <c r="C79" t="n">
-        <v>-91.732021</v>
+        <v>-137.23466</v>
       </c>
       <c r="D79" t="n">
-        <v>-5.8913638</v>
+        <v>0.0089554649</v>
       </c>
       <c r="E79" t="n">
         <v>0</v>
@@ -3147,13 +3147,13 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>175</v>
+        <v>500</v>
       </c>
       <c r="C80" t="n">
-        <v>-41.25803</v>
+        <v>-162.31879</v>
       </c>
       <c r="D80" t="n">
-        <v>-5.4823388</v>
+        <v>0.0059283152</v>
       </c>
       <c r="E80" t="n">
         <v>0</v>
@@ -3170,10 +3170,10 @@
         <v>175</v>
       </c>
       <c r="C81" t="n">
-        <v>-50.509948</v>
+        <v>24.990052</v>
       </c>
       <c r="D81" t="n">
-        <v>-4.7374183</v>
+        <v>1.2938696</v>
       </c>
       <c r="E81" t="n">
         <v>0</v>
@@ -3190,10 +3190,10 @@
         <v>175</v>
       </c>
       <c r="C82" t="n">
-        <v>-21.5</v>
+        <v>-91.732021</v>
       </c>
       <c r="D82" t="n">
-        <v>24.906579</v>
+        <v>-5.8913638</v>
       </c>
       <c r="E82" t="n">
         <v>0</v>
@@ -3210,10 +3210,10 @@
         <v>175</v>
       </c>
       <c r="C83" t="n">
-        <v>2.8699097</v>
+        <v>-41.25803</v>
       </c>
       <c r="D83" t="n">
-        <v>-1.4316455</v>
+        <v>-5.4823388</v>
       </c>
       <c r="E83" t="n">
         <v>0</v>
@@ -3227,13 +3227,13 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>400</v>
+        <v>175</v>
       </c>
       <c r="C84" t="n">
-        <v>-274.60193</v>
+        <v>-50.509948</v>
       </c>
       <c r="D84" t="n">
-        <v>-1.3348037</v>
+        <v>-4.7374183</v>
       </c>
       <c r="E84" t="n">
         <v>0</v>
@@ -3250,10 +3250,10 @@
         <v>175</v>
       </c>
       <c r="C85" t="n">
-        <v>-124.50995</v>
+        <v>-21.5</v>
       </c>
       <c r="D85" t="n">
-        <v>-3.8794607</v>
+        <v>24.906579</v>
       </c>
       <c r="E85" t="n">
         <v>0</v>
@@ -3270,10 +3270,10 @@
         <v>175</v>
       </c>
       <c r="C86" t="n">
-        <v>-112.25803</v>
+        <v>2.8699097</v>
       </c>
       <c r="D86" t="n">
-        <v>-5.6758331</v>
+        <v>-1.4316455</v>
       </c>
       <c r="E86" t="n">
         <v>0</v>
@@ -3287,16 +3287,16 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>175</v>
+        <v>400</v>
       </c>
       <c r="C87" t="n">
-        <v>-157.5</v>
+        <v>-274.60193</v>
       </c>
       <c r="D87" t="n">
-        <v>7.9130277</v>
+        <v>-1.3348037</v>
       </c>
       <c r="E87" t="n">
-        <v>45.271648</v>
+        <v>0</v>
       </c>
       <c r="F87" t="n">
         <v>0</v>
@@ -3310,10 +3310,10 @@
         <v>175</v>
       </c>
       <c r="C88" t="n">
-        <v>44.239137</v>
+        <v>-124.50995</v>
       </c>
       <c r="D88" t="n">
-        <v>0</v>
+        <v>-3.8794607</v>
       </c>
       <c r="E88" t="n">
         <v>0</v>
@@ -3330,10 +3330,10 @@
         <v>175</v>
       </c>
       <c r="C89" t="n">
-        <v>-80.43588</v>
+        <v>-112.25803</v>
       </c>
       <c r="D89" t="n">
-        <v>1.9175813</v>
+        <v>-5.6758331</v>
       </c>
       <c r="E89" t="n">
         <v>0</v>
@@ -3350,13 +3350,13 @@
         <v>175</v>
       </c>
       <c r="C90" t="n">
-        <v>-46.324983</v>
+        <v>-157.5</v>
       </c>
       <c r="D90" t="n">
-        <v>-1.9175813</v>
+        <v>7.9130277</v>
       </c>
       <c r="E90" t="n">
-        <v>0</v>
+        <v>45.271648</v>
       </c>
       <c r="F90" t="n">
         <v>0</v>
@@ -3367,13 +3367,13 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>400</v>
+        <v>175</v>
       </c>
       <c r="C91" t="n">
-        <v>-168.8819</v>
+        <v>44.239137</v>
       </c>
       <c r="D91" t="n">
-        <v>-1.5676448</v>
+        <v>0</v>
       </c>
       <c r="E91" t="n">
         <v>0</v>
@@ -3387,13 +3387,13 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>400</v>
+        <v>175</v>
       </c>
       <c r="C92" t="n">
-        <v>-208.19402</v>
+        <v>-80.43588</v>
       </c>
       <c r="D92" t="n">
-        <v>-1.6001159</v>
+        <v>1.9175813</v>
       </c>
       <c r="E92" t="n">
         <v>0</v>
@@ -3407,13 +3407,13 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>400</v>
+        <v>175</v>
       </c>
       <c r="C93" t="n">
-        <v>-235.88545</v>
+        <v>-46.324983</v>
       </c>
       <c r="D93" t="n">
-        <v>2.2675178</v>
+        <v>-1.9175813</v>
       </c>
       <c r="E93" t="n">
         <v>0</v>
@@ -3430,10 +3430,10 @@
         <v>400</v>
       </c>
       <c r="C94" t="n">
-        <v>-275.19757</v>
+        <v>-168.8819</v>
       </c>
       <c r="D94" t="n">
-        <v>2.2350466</v>
+        <v>-1.5676448</v>
       </c>
       <c r="E94" t="n">
         <v>0</v>
@@ -3447,13 +3447,13 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="C95" t="n">
-        <v>-285.9301</v>
+        <v>-208.19402</v>
       </c>
       <c r="D95" t="n">
-        <v>0.08670847</v>
+        <v>-1.6001159</v>
       </c>
       <c r="E95" t="n">
         <v>0</v>
@@ -3467,13 +3467,13 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="C96" t="n">
-        <v>-118.83724</v>
+        <v>-235.88545</v>
       </c>
       <c r="D96" t="n">
-        <v>0.27406659</v>
+        <v>2.2675178</v>
       </c>
       <c r="E96" t="n">
         <v>0</v>
@@ -3487,13 +3487,13 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="C97" t="n">
-        <v>-217.1339</v>
+        <v>-275.19757</v>
       </c>
       <c r="D97" t="n">
-        <v>0.1191796</v>
+        <v>2.2350466</v>
       </c>
       <c r="E97" t="n">
         <v>0</v>
@@ -3510,10 +3510,10 @@
         <v>500</v>
       </c>
       <c r="C98" t="n">
-        <v>-266.25768</v>
+        <v>-285.9301</v>
       </c>
       <c r="D98" t="n">
-        <v>0.49235173</v>
+        <v>0.08670847</v>
       </c>
       <c r="E98" t="n">
         <v>0</v>
@@ -3530,10 +3530,10 @@
         <v>500</v>
       </c>
       <c r="C99" t="n">
-        <v>-177.064</v>
+        <v>-118.83724</v>
       </c>
       <c r="D99" t="n">
-        <v>0.37317213</v>
+        <v>0.27406659</v>
       </c>
       <c r="E99" t="n">
         <v>0</v>
@@ -3550,10 +3550,10 @@
         <v>500</v>
       </c>
       <c r="C100" t="n">
-        <v>-312.83724</v>
+        <v>-217.1339</v>
       </c>
       <c r="D100" t="n">
-        <v>0.38499831</v>
+        <v>0.1191796</v>
       </c>
       <c r="E100" t="n">
         <v>0</v>
@@ -3570,10 +3570,10 @@
         <v>500</v>
       </c>
       <c r="C101" t="n">
-        <v>3.1023958</v>
+        <v>-266.25768</v>
       </c>
       <c r="D101" t="n">
-        <v>-0.17911456</v>
+        <v>0.49235173</v>
       </c>
       <c r="E101" t="n">
         <v>0</v>
@@ -3590,10 +3590,10 @@
         <v>500</v>
       </c>
       <c r="C102" t="n">
-        <v>-219.85216</v>
+        <v>-177.064</v>
       </c>
       <c r="D102" t="n">
-        <v>-0.13118207</v>
+        <v>0.37317213</v>
       </c>
       <c r="E102" t="n">
         <v>0</v>
@@ -3610,10 +3610,10 @@
         <v>500</v>
       </c>
       <c r="C103" t="n">
-        <v>-219.85216</v>
+        <v>-312.83724</v>
       </c>
       <c r="D103" t="n">
-        <v>-0.13118207</v>
+        <v>0.38499831</v>
       </c>
       <c r="E103" t="n">
         <v>0</v>
@@ -3630,10 +3630,10 @@
         <v>500</v>
       </c>
       <c r="C104" t="n">
-        <v>274.60193</v>
+        <v>3.1023958</v>
       </c>
       <c r="D104" t="n">
-        <v>0.82630708</v>
+        <v>-0.17911456</v>
       </c>
       <c r="E104" t="n">
         <v>0</v>
@@ -3650,10 +3650,10 @@
         <v>500</v>
       </c>
       <c r="C105" t="n">
-        <v>-279.51907</v>
+        <v>-219.85216</v>
       </c>
       <c r="D105" t="n">
-        <v>-0.0083760876</v>
+        <v>-0.13118207</v>
       </c>
       <c r="E105" t="n">
         <v>0</v>
@@ -3670,10 +3670,10 @@
         <v>500</v>
       </c>
       <c r="C106" t="n">
-        <v>24.784226</v>
+        <v>-219.85216</v>
       </c>
       <c r="D106" t="n">
-        <v>-0.084837758</v>
+        <v>-0.13118207</v>
       </c>
       <c r="E106" t="n">
         <v>0</v>
@@ -3690,10 +3690,10 @@
         <v>500</v>
       </c>
       <c r="C107" t="n">
-        <v>-141.03352</v>
+        <v>274.60193</v>
       </c>
       <c r="D107" t="n">
-        <v>-0.009066964</v>
+        <v>0.82630708</v>
       </c>
       <c r="E107" t="n">
         <v>0</v>
@@ -3710,10 +3710,10 @@
         <v>500</v>
       </c>
       <c r="C108" t="n">
-        <v>-138.48555</v>
+        <v>-279.51907</v>
       </c>
       <c r="D108" t="n">
-        <v>0.034175722</v>
+        <v>-0.0083760876</v>
       </c>
       <c r="E108" t="n">
         <v>0</v>
@@ -3730,10 +3730,10 @@
         <v>500</v>
       </c>
       <c r="C109" t="n">
-        <v>-60.90506</v>
+        <v>24.784226</v>
       </c>
       <c r="D109" t="n">
-        <v>0.065375535</v>
+        <v>-0.084837758</v>
       </c>
       <c r="E109" t="n">
         <v>0</v>
@@ -3750,10 +3750,10 @@
         <v>500</v>
       </c>
       <c r="C110" t="n">
-        <v>-60.90506</v>
+        <v>-141.03352</v>
       </c>
       <c r="D110" t="n">
-        <v>0.065375535</v>
+        <v>-0.009066964</v>
       </c>
       <c r="E110" t="n">
         <v>0</v>
@@ -3770,10 +3770,10 @@
         <v>500</v>
       </c>
       <c r="C111" t="n">
-        <v>-78.10788700000001</v>
+        <v>-138.48555</v>
       </c>
       <c r="D111" t="n">
-        <v>-0.073771964</v>
+        <v>0.034175722</v>
       </c>
       <c r="E111" t="n">
         <v>0</v>
@@ -3790,10 +3790,10 @@
         <v>500</v>
       </c>
       <c r="C112" t="n">
-        <v>-78.10788700000001</v>
+        <v>-60.90506</v>
       </c>
       <c r="D112" t="n">
-        <v>-0.073771964</v>
+        <v>0.065375535</v>
       </c>
       <c r="E112" t="n">
         <v>0</v>
@@ -3810,10 +3810,10 @@
         <v>500</v>
       </c>
       <c r="C113" t="n">
-        <v>-142.10789</v>
+        <v>-60.90506</v>
       </c>
       <c r="D113" t="n">
-        <v>-0.04057458</v>
+        <v>0.065375535</v>
       </c>
       <c r="E113" t="n">
         <v>0</v>
@@ -3830,10 +3830,10 @@
         <v>500</v>
       </c>
       <c r="C114" t="n">
-        <v>-142.10789</v>
+        <v>-78.10788700000001</v>
       </c>
       <c r="D114" t="n">
-        <v>-0.04057458</v>
+        <v>-0.073771964</v>
       </c>
       <c r="E114" t="n">
         <v>0</v>
@@ -3850,10 +3850,10 @@
         <v>500</v>
       </c>
       <c r="C115" t="n">
-        <v>-161.51445</v>
+        <v>-78.10788700000001</v>
       </c>
       <c r="D115" t="n">
-        <v>-0.022132849</v>
+        <v>-0.073771964</v>
       </c>
       <c r="E115" t="n">
         <v>0</v>
@@ -3867,13 +3867,13 @@
         <v>114</v>
       </c>
       <c r="B116" t="n">
-        <v>722</v>
+        <v>500</v>
       </c>
       <c r="C116" t="n">
-        <v>-67.537462</v>
+        <v>-142.10789</v>
       </c>
       <c r="D116" t="n">
-        <v>0.051088748</v>
+        <v>-0.04057458</v>
       </c>
       <c r="E116" t="n">
         <v>0</v>
@@ -3887,13 +3887,13 @@
         <v>115</v>
       </c>
       <c r="B117" t="n">
-        <v>175</v>
+        <v>500</v>
       </c>
       <c r="C117" t="n">
-        <v>3.6946489</v>
+        <v>-142.10789</v>
       </c>
       <c r="D117" t="n">
-        <v>0.35499614</v>
+        <v>-0.04057458</v>
       </c>
       <c r="E117" t="n">
         <v>0</v>
@@ -3907,13 +3907,13 @@
         <v>116</v>
       </c>
       <c r="B118" t="n">
-        <v>175</v>
+        <v>500</v>
       </c>
       <c r="C118" t="n">
-        <v>-3.6946489</v>
+        <v>-161.51445</v>
       </c>
       <c r="D118" t="n">
-        <v>-0.35499614</v>
+        <v>-0.022132849</v>
       </c>
       <c r="E118" t="n">
         <v>0</v>
@@ -3930,10 +3930,10 @@
         <v>500</v>
       </c>
       <c r="C119" t="n">
-        <v>-49.686438</v>
+        <v>-67.537462</v>
       </c>
       <c r="D119" t="n">
-        <v>0.11819866</v>
+        <v>0.55062318</v>
       </c>
       <c r="E119" t="n">
         <v>0</v>
@@ -3950,10 +3950,10 @@
         <v>500</v>
       </c>
       <c r="C120" t="n">
-        <v>49.686438</v>
+        <v>47.776599</v>
       </c>
       <c r="D120" t="n">
-        <v>-0.11819866</v>
+        <v>-0.59035887</v>
       </c>
       <c r="E120" t="n">
         <v>0</v>
@@ -3967,118 +3967,18 @@
         <v>119</v>
       </c>
       <c r="B121" t="n">
-        <v>500</v>
+        <v>722</v>
       </c>
       <c r="C121" t="n">
-        <v>7.2865617</v>
+        <v>-67.537462</v>
       </c>
       <c r="D121" t="n">
-        <v>-0.069757085</v>
+        <v>0.051088748</v>
       </c>
       <c r="E121" t="n">
         <v>0</v>
       </c>
       <c r="F121" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122" s="1" t="n">
-        <v>120</v>
-      </c>
-      <c r="B122" t="n">
-        <v>500</v>
-      </c>
-      <c r="C122" t="n">
-        <v>-7.2865617</v>
-      </c>
-      <c r="D122" t="n">
-        <v>0.069757085</v>
-      </c>
-      <c r="E122" t="n">
-        <v>0</v>
-      </c>
-      <c r="F122" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="123">
-      <c r="A123" s="1" t="n">
-        <v>121</v>
-      </c>
-      <c r="B123" t="n">
-        <v>500</v>
-      </c>
-      <c r="C123" t="n">
-        <v>-67.537462</v>
-      </c>
-      <c r="D123" t="n">
-        <v>0.27531159</v>
-      </c>
-      <c r="E123" t="n">
-        <v>0</v>
-      </c>
-      <c r="F123" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="124">
-      <c r="A124" s="1" t="n">
-        <v>122</v>
-      </c>
-      <c r="B124" t="n">
-        <v>500</v>
-      </c>
-      <c r="C124" t="n">
-        <v>67.537462</v>
-      </c>
-      <c r="D124" t="n">
-        <v>-0.27531159</v>
-      </c>
-      <c r="E124" t="n">
-        <v>0</v>
-      </c>
-      <c r="F124" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="125">
-      <c r="A125" s="1" t="n">
-        <v>123</v>
-      </c>
-      <c r="B125" t="n">
-        <v>500</v>
-      </c>
-      <c r="C125" t="n">
-        <v>47.776599</v>
-      </c>
-      <c r="D125" t="n">
-        <v>-0.29517943</v>
-      </c>
-      <c r="E125" t="n">
-        <v>0</v>
-      </c>
-      <c r="F125" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="126">
-      <c r="A126" s="1" t="n">
-        <v>124</v>
-      </c>
-      <c r="B126" t="n">
-        <v>500</v>
-      </c>
-      <c r="C126" t="n">
-        <v>-47.776599</v>
-      </c>
-      <c r="D126" t="n">
-        <v>0.29517943</v>
-      </c>
-      <c r="E126" t="n">
-        <v>0</v>
-      </c>
-      <c r="F126" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4093,7 +3993,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C79"/>
+  <dimension ref="A1:C74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4916,61 +4816,6 @@
         <v>0.57666027</v>
       </c>
     </row>
-    <row r="75">
-      <c r="A75" s="1" t="n">
-        <v>73</v>
-      </c>
-      <c r="B75" t="n">
-        <v>100.355</v>
-      </c>
-      <c r="C75" t="n">
-        <v>0.13743732</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" s="1" t="n">
-        <v>74</v>
-      </c>
-      <c r="B76" t="n">
-        <v>100.24036</v>
-      </c>
-      <c r="C76" t="n">
-        <v>0.48426462</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="B77" t="n">
-        <v>100.45922</v>
-      </c>
-      <c r="C77" t="n">
-        <v>0.58666125</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" s="1" t="n">
-        <v>76</v>
-      </c>
-      <c r="B78" t="n">
-        <v>101.13622</v>
-      </c>
-      <c r="C78" t="n">
-        <v>0.6094159300000001</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" s="1" t="n">
-        <v>77</v>
-      </c>
-      <c r="B79" t="n">
-        <v>100.69638</v>
-      </c>
-      <c r="C79" t="n">
-        <v>0.5813512</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>